<commit_message>
Update InsideBet Data: Automatizado
</commit_message>
<xml_diff>
--- a/datos_fbref/CARTELERA_PROXIMOS_Bundesliga.xlsx
+++ b/datos_fbref/CARTELERA_PROXIMOS_Bundesliga.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,34 +813,34 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-21</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>20:30 (16:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Mewa Arena</t>
+          <t>Volkswagen Arena</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -874,19 +874,19 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Köln</t>
         </is>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Volkswagen Arena</t>
+          <t>RheinEnergieSTADION</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
@@ -920,19 +920,19 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>RheinEnergieSTADION</t>
+          <t>Stadion An der Alten Försterei</t>
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
@@ -966,19 +966,19 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Stadion An der Alten Försterei</t>
+          <t>Allianz Arena</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
@@ -1007,24 +1007,24 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>18:30 (14:30)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Allianz Arena</t>
+          <t>Red Bull Arena</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
@@ -1043,34 +1043,34 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2026-02-21</t>
+          <t>2026-02-22</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>18:30 (14:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Red Bull Arena</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
@@ -1099,24 +1099,24 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>17:30 (13:30)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Europa-Park Stadion</t>
+          <t>Millerntor-Stadion</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
@@ -1145,24 +1145,24 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>17:30 (13:30)</t>
+          <t>19:30 (15:30)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>Voith-Arena</t>
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
@@ -1174,63 +1174,63 @@
       <c r="L32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Sun</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>2026-02-22</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>19:30 (15:30)</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Heidenheim</t>
-        </is>
-      </c>
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Stuttgart</t>
-        </is>
-      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Voith-Arena</t>
-        </is>
-      </c>
+      <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>20:30 (16:30)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Augsburg</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Köln</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>WWK Arena</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L34" t="inlineStr"/>
     </row>
     <row r="35">
@@ -1241,34 +1241,34 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2026-02-27</t>
+          <t>2026-02-28</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>20:30 (16:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr">
         <is>
-          <t>WWK Arena</t>
+          <t>Weserstadion</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
@@ -1302,19 +1302,19 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Weserstadion</t>
+          <t>BayArena</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
@@ -1348,19 +1348,19 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>BayArena</t>
+          <t>PreZero Arena</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -1394,19 +1394,19 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
-          <t>PreZero Arena</t>
+          <t>Stadion im Borussia-Park</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -1435,24 +1435,24 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>18:30 (14:30)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Stadion im Borussia-Park</t>
+          <t>Signal Iduna Park</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -1471,34 +1471,34 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2026-02-28</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>18:30 (14:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Signal Iduna Park</t>
+          <t>MHPArena</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -1527,24 +1527,24 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>17:30 (13:30)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
-          <t>MHPArena</t>
+          <t>Deutsche Bank Park</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
@@ -1573,24 +1573,24 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>17:30 (13:30)</t>
+          <t>19:30 (15:30)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Deutsche Bank Park</t>
+          <t>Volksparkstadion</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -1602,123 +1602,123 @@
       <c r="L42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Sun</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>2026-03-01</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>19:30 (15:30)</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2026-03-04</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>20:30 (16:30)</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>Hamburger SV</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>RB Leipzig</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr">
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
         <is>
           <t>Volksparkstadion</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>2026-03-04</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2026-03-06</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
         <is>
           <t>20:30 (16:30)</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Hamburger SV</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Leverkusen</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>Volksparkstadion</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr"/>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Bayern Munich</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Gladbach</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Allianz Arena</t>
+        </is>
+      </c>
       <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L46" t="inlineStr"/>
     </row>
     <row r="47">
@@ -1729,34 +1729,34 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2026-03-06</t>
+          <t>2026-03-07</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>20:30 (16:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Allianz Arena</t>
+          <t>Mewa Arena</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -1790,19 +1790,19 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Mewa Arena</t>
+          <t>Red Bull Arena</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
@@ -1836,19 +1836,19 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Red Bull Arena</t>
+          <t>Voith-Arena</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -1882,19 +1882,19 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Voith-Arena</t>
+          <t>Volkswagen Arena</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -1928,19 +1928,19 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Volkswagen Arena</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -1969,24 +1969,24 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>18:30 (14:30)</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Köln</t>
         </is>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Europa-Park Stadion</t>
+          <t>RheinEnergieSTADION</t>
         </is>
       </c>
       <c r="J52" t="inlineStr"/>
@@ -2005,34 +2005,34 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2026-03-07</t>
+          <t>2026-03-08</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>18:30 (14:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
         <is>
-          <t>RheinEnergieSTADION</t>
+          <t>Millerntor-Stadion</t>
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
@@ -2061,24 +2061,24 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>17:30 (13:30)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>Stadion An der Alten Försterei</t>
         </is>
       </c>
       <c r="J54" t="inlineStr"/>
@@ -2090,63 +2090,63 @@
       <c r="L54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Sun</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>2026-03-08</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>17:30 (13:30)</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Union Berlin</t>
-        </is>
-      </c>
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Werder Bremen</t>
-        </is>
-      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>Stadion An der Alten Försterei</t>
-        </is>
-      </c>
+      <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2026-03-13</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>20:30 (16:30)</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Gladbach</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>St Pauli</t>
+        </is>
+      </c>
       <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Stadion im Borussia-Park</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -2157,34 +2157,34 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2026-03-13</t>
+          <t>2026-03-14</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>20:30 (16:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Stadion im Borussia-Park</t>
+          <t>BayArena</t>
         </is>
       </c>
       <c r="J57" t="inlineStr"/>
@@ -2218,19 +2218,19 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
-          <t>BayArena</t>
+          <t>Deutsche Bank Park</t>
         </is>
       </c>
       <c r="J58" t="inlineStr"/>
@@ -2264,19 +2264,19 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Deutsche Bank Park</t>
+          <t>PreZero Arena</t>
         </is>
       </c>
       <c r="J59" t="inlineStr"/>
@@ -2310,19 +2310,19 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
-          <t>PreZero Arena</t>
+          <t>Signal Iduna Park</t>
         </is>
       </c>
       <c r="J60" t="inlineStr"/>
@@ -2351,24 +2351,24 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>18:30 (14:30)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Köln</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Signal Iduna Park</t>
+          <t>Volksparkstadion</t>
         </is>
       </c>
       <c r="J61" t="inlineStr"/>
@@ -2387,34 +2387,34 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2026-03-14</t>
+          <t>2026-03-15</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>18:30 (14:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Volksparkstadion</t>
+          <t>Weserstadion</t>
         </is>
       </c>
       <c r="J62" t="inlineStr"/>
@@ -2443,24 +2443,24 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>17:30 (13:30)</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Weserstadion</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
@@ -2489,24 +2489,24 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>17:30 (13:30)</t>
+          <t>19:30 (15:30)</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Europa-Park Stadion</t>
+          <t>MHPArena</t>
         </is>
       </c>
       <c r="J64" t="inlineStr"/>
@@ -2518,63 +2518,63 @@
       <c r="L64" t="inlineStr"/>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Sun</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>2026-03-15</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>19:30 (15:30)</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>Stuttgart</t>
-        </is>
-      </c>
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr">
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2026-03-20</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>20:30 (16:30)</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>RB Leipzig</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>MHPArena</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr"/>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Red Bull Arena</t>
+        </is>
+      </c>
       <c r="J66" t="inlineStr"/>
-      <c r="K66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L66" t="inlineStr"/>
     </row>
     <row r="67">
@@ -2585,34 +2585,34 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2026-03-20</t>
+          <t>2026-03-21</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>20:30 (16:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Köln</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr">
         <is>
-          <t>Red Bull Arena</t>
+          <t>RheinEnergieSTADION</t>
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
@@ -2646,19 +2646,19 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
         <is>
-          <t>RheinEnergieSTADION</t>
+          <t>Volkswagen Arena</t>
         </is>
       </c>
       <c r="J68" t="inlineStr"/>
@@ -2692,19 +2692,19 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
         <is>
-          <t>Volkswagen Arena</t>
+          <t>Allianz Arena</t>
         </is>
       </c>
       <c r="J69" t="inlineStr"/>
@@ -2738,19 +2738,19 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr">
         <is>
-          <t>Allianz Arena</t>
+          <t>Voith-Arena</t>
         </is>
       </c>
       <c r="J70" t="inlineStr"/>
@@ -2779,24 +2779,24 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>18:30 (14:30)</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr">
         <is>
-          <t>Voith-Arena</t>
+          <t>Signal Iduna Park</t>
         </is>
       </c>
       <c r="J71" t="inlineStr"/>
@@ -2815,34 +2815,34 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2026-03-21</t>
+          <t>2026-03-22</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>18:30 (14:30)</t>
+          <t>15:30 (11:30)</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr">
         <is>
-          <t>Signal Iduna Park</t>
+          <t>Mewa Arena</t>
         </is>
       </c>
       <c r="J72" t="inlineStr"/>
@@ -2871,24 +2871,24 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15:30 (11:30)</t>
+          <t>17:30 (13:30)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr">
         <is>
-          <t>Mewa Arena</t>
+          <t>Millerntor-Stadion</t>
         </is>
       </c>
       <c r="J73" t="inlineStr"/>
@@ -2917,24 +2917,24 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>17:30 (13:30)</t>
+          <t>19:30 (15:30)</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>WWK Arena</t>
         </is>
       </c>
       <c r="J74" t="inlineStr"/>
@@ -2946,63 +2946,59 @@
       <c r="L74" t="inlineStr"/>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Sun</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>2026-03-22</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>19:30 (15:30)</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Augsburg</t>
-        </is>
-      </c>
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>Stuttgart</t>
-        </is>
-      </c>
+      <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>WWK Arena</t>
-        </is>
-      </c>
+      <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2026-04-04</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Köln</t>
+        </is>
+      </c>
       <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr"/>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Deutsche Bank Park</t>
+        </is>
+      </c>
       <c r="J76" t="inlineStr"/>
-      <c r="K76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L76" t="inlineStr"/>
     </row>
     <row r="77">
@@ -3024,19 +3020,19 @@
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
         <is>
-          <t>Deutsche Bank Park</t>
+          <t>Stadion im Borussia-Park</t>
         </is>
       </c>
       <c r="J77" t="inlineStr"/>
@@ -3066,19 +3062,19 @@
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr">
         <is>
-          <t>Stadion im Borussia-Park</t>
+          <t>MHPArena</t>
         </is>
       </c>
       <c r="J78" t="inlineStr"/>
@@ -3108,19 +3104,19 @@
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr">
         <is>
-          <t>MHPArena</t>
+          <t>Stadion An der Alten Försterei</t>
         </is>
       </c>
       <c r="J79" t="inlineStr"/>
@@ -3150,19 +3146,19 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr">
         <is>
-          <t>Stadion An der Alten Försterei</t>
+          <t>PreZero Arena</t>
         </is>
       </c>
       <c r="J80" t="inlineStr"/>
@@ -3192,19 +3188,19 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr">
         <is>
-          <t>PreZero Arena</t>
+          <t>Weserstadion</t>
         </is>
       </c>
       <c r="J81" t="inlineStr"/>
@@ -3234,19 +3230,19 @@
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr">
         <is>
-          <t>Weserstadion</t>
+          <t>Volksparkstadion</t>
         </is>
       </c>
       <c r="J82" t="inlineStr"/>
@@ -3276,19 +3272,19 @@
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr">
         <is>
-          <t>Volksparkstadion</t>
+          <t>BayArena</t>
         </is>
       </c>
       <c r="J83" t="inlineStr"/>
@@ -3318,19 +3314,19 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr">
         <is>
-          <t>BayArena</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J84" t="inlineStr"/>
@@ -3342,59 +3338,59 @@
       <c r="L84" t="inlineStr"/>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>2026-04-04</t>
-        </is>
-      </c>
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Freiburg</t>
-        </is>
-      </c>
+      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Bayern Munich</t>
-        </is>
-      </c>
+      <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>Europa-Park Stadion</t>
-        </is>
-      </c>
+      <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr"/>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2026-04-11</t>
+        </is>
+      </c>
       <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Köln</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Werder Bremen</t>
+        </is>
+      </c>
       <c r="H86" t="inlineStr"/>
-      <c r="I86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>RheinEnergieSTADION</t>
+        </is>
+      </c>
       <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L86" t="inlineStr"/>
     </row>
     <row r="87">
@@ -3416,19 +3412,19 @@
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr">
         <is>
-          <t>RheinEnergieSTADION</t>
+          <t>Volkswagen Arena</t>
         </is>
       </c>
       <c r="J87" t="inlineStr"/>
@@ -3458,19 +3454,19 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr">
         <is>
-          <t>Volkswagen Arena</t>
+          <t>Millerntor-Stadion</t>
         </is>
       </c>
       <c r="J88" t="inlineStr"/>
@@ -3500,19 +3496,19 @@
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>WWK Arena</t>
         </is>
       </c>
       <c r="J89" t="inlineStr"/>
@@ -3542,19 +3538,19 @@
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr">
         <is>
-          <t>WWK Arena</t>
+          <t>Red Bull Arena</t>
         </is>
       </c>
       <c r="J90" t="inlineStr"/>
@@ -3584,19 +3580,19 @@
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr">
         <is>
-          <t>Red Bull Arena</t>
+          <t>Signal Iduna Park</t>
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
@@ -3626,19 +3622,19 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
-          <t>Signal Iduna Park</t>
+          <t>Mewa Arena</t>
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
@@ -3668,19 +3664,19 @@
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
-          <t>Mewa Arena</t>
+          <t>Voith-Arena</t>
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
@@ -3710,19 +3706,19 @@
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr">
         <is>
-          <t>Voith-Arena</t>
+          <t>MHPArena</t>
         </is>
       </c>
       <c r="J94" t="inlineStr"/>
@@ -3734,59 +3730,59 @@
       <c r="L94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>2026-04-11</t>
-        </is>
-      </c>
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Stuttgart</t>
-        </is>
-      </c>
+      <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Hamburger SV</t>
-        </is>
-      </c>
+      <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>MHPArena</t>
-        </is>
-      </c>
+      <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr"/>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2026-04-18</t>
+        </is>
+      </c>
       <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
       <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Dortmund</t>
+        </is>
+      </c>
       <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr"/>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>PreZero Arena</t>
+        </is>
+      </c>
       <c r="J96" t="inlineStr"/>
-      <c r="K96" t="inlineStr"/>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L96" t="inlineStr"/>
     </row>
     <row r="97">
@@ -3808,19 +3804,19 @@
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="inlineStr">
         <is>
-          <t>PreZero Arena</t>
+          <t>Weserstadion</t>
         </is>
       </c>
       <c r="J97" t="inlineStr"/>
@@ -3850,19 +3846,19 @@
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr">
         <is>
-          <t>Weserstadion</t>
+          <t>BayArena</t>
         </is>
       </c>
       <c r="J98" t="inlineStr"/>
@@ -3892,19 +3888,19 @@
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr">
         <is>
-          <t>BayArena</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J99" t="inlineStr"/>
@@ -3934,19 +3930,19 @@
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr">
         <is>
-          <t>Europa-Park Stadion</t>
+          <t>Deutsche Bank Park</t>
         </is>
       </c>
       <c r="J100" t="inlineStr"/>
@@ -3976,19 +3972,19 @@
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Köln</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
       <c r="I101" t="inlineStr">
         <is>
-          <t>Deutsche Bank Park</t>
+          <t>Millerntor-Stadion</t>
         </is>
       </c>
       <c r="J101" t="inlineStr"/>
@@ -4018,19 +4014,19 @@
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
       <c r="I102" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>Stadion im Borussia-Park</t>
         </is>
       </c>
       <c r="J102" t="inlineStr"/>
@@ -4060,19 +4056,19 @@
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr">
         <is>
-          <t>Stadion im Borussia-Park</t>
+          <t>Stadion An der Alten Försterei</t>
         </is>
       </c>
       <c r="J103" t="inlineStr"/>
@@ -4102,19 +4098,19 @@
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr">
         <is>
-          <t>Stadion An der Alten Försterei</t>
+          <t>Allianz Arena</t>
         </is>
       </c>
       <c r="J104" t="inlineStr"/>
@@ -4126,59 +4122,59 @@
       <c r="L104" t="inlineStr"/>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>2026-04-18</t>
-        </is>
-      </c>
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>Bayern Munich</t>
-        </is>
-      </c>
+      <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>Stuttgart</t>
-        </is>
-      </c>
+      <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>Allianz Arena</t>
-        </is>
-      </c>
+      <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2026-04-25</t>
+        </is>
+      </c>
       <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Köln</t>
+        </is>
+      </c>
       <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Leverkusen</t>
+        </is>
+      </c>
       <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr"/>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>RheinEnergieSTADION</t>
+        </is>
+      </c>
       <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr"/>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L106" t="inlineStr"/>
     </row>
     <row r="107">
@@ -4200,19 +4196,19 @@
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr">
         <is>
-          <t>RheinEnergieSTADION</t>
+          <t>Volkswagen Arena</t>
         </is>
       </c>
       <c r="J107" t="inlineStr"/>
@@ -4242,19 +4238,19 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr">
         <is>
-          <t>Volkswagen Arena</t>
+          <t>Signal Iduna Park</t>
         </is>
       </c>
       <c r="J108" t="inlineStr"/>
@@ -4284,19 +4280,19 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr">
         <is>
-          <t>Signal Iduna Park</t>
+          <t>MHPArena</t>
         </is>
       </c>
       <c r="J109" t="inlineStr"/>
@@ -4326,19 +4322,19 @@
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr">
         <is>
-          <t>MHPArena</t>
+          <t>WWK Arena</t>
         </is>
       </c>
       <c r="J110" t="inlineStr"/>
@@ -4368,19 +4364,19 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
       <c r="I111" t="inlineStr">
         <is>
-          <t>WWK Arena</t>
+          <t>Red Bull Arena</t>
         </is>
       </c>
       <c r="J111" t="inlineStr"/>
@@ -4410,19 +4406,19 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr">
         <is>
-          <t>Red Bull Arena</t>
+          <t>Mewa Arena</t>
         </is>
       </c>
       <c r="J112" t="inlineStr"/>
@@ -4452,19 +4448,19 @@
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="H113" t="inlineStr"/>
       <c r="I113" t="inlineStr">
         <is>
-          <t>Mewa Arena</t>
+          <t>Voith-Arena</t>
         </is>
       </c>
       <c r="J113" t="inlineStr"/>
@@ -4494,19 +4490,19 @@
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr">
         <is>
-          <t>Voith-Arena</t>
+          <t>Volksparkstadion</t>
         </is>
       </c>
       <c r="J114" t="inlineStr"/>
@@ -4518,59 +4514,59 @@
       <c r="L114" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>2026-04-25</t>
-        </is>
-      </c>
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>Hamburger SV</t>
-        </is>
-      </c>
+      <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>Hoffenheim</t>
-        </is>
-      </c>
+      <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>Volksparkstadion</t>
-        </is>
-      </c>
+      <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr"/>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr"/>
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2026-05-02</t>
+        </is>
+      </c>
       <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Union Berlin</t>
+        </is>
+      </c>
       <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr"/>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Köln</t>
+        </is>
+      </c>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr"/>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Stadion An der Alten Försterei</t>
+        </is>
+      </c>
       <c r="J116" t="inlineStr"/>
-      <c r="K116" t="inlineStr"/>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L116" t="inlineStr"/>
     </row>
     <row r="117">
@@ -4592,19 +4588,19 @@
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr">
         <is>
-          <t>Stadion An der Alten Försterei</t>
+          <t>Allianz Arena</t>
         </is>
       </c>
       <c r="J117" t="inlineStr"/>
@@ -4634,19 +4630,19 @@
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="inlineStr">
         <is>
-          <t>Allianz Arena</t>
+          <t>PreZero Arena</t>
         </is>
       </c>
       <c r="J118" t="inlineStr"/>
@@ -4676,19 +4672,19 @@
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="inlineStr">
         <is>
-          <t>PreZero Arena</t>
+          <t>Stadion im Borussia-Park</t>
         </is>
       </c>
       <c r="J119" t="inlineStr"/>
@@ -4718,19 +4714,19 @@
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
       <c r="I120" t="inlineStr">
         <is>
-          <t>Stadion im Borussia-Park</t>
+          <t>BayArena</t>
         </is>
       </c>
       <c r="J120" t="inlineStr"/>
@@ -4760,19 +4756,19 @@
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F121" t="inlineStr"/>
       <c r="G121" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
       <c r="I121" t="inlineStr">
         <is>
-          <t>BayArena</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J121" t="inlineStr"/>
@@ -4802,19 +4798,19 @@
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="F122" t="inlineStr"/>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr">
         <is>
-          <t>Europa-Park Stadion</t>
+          <t>Weserstadion</t>
         </is>
       </c>
       <c r="J122" t="inlineStr"/>
@@ -4844,19 +4840,19 @@
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="F123" t="inlineStr"/>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="H123" t="inlineStr"/>
       <c r="I123" t="inlineStr">
         <is>
-          <t>Weserstadion</t>
+          <t>Millerntor-Stadion</t>
         </is>
       </c>
       <c r="J123" t="inlineStr"/>
@@ -4886,19 +4882,19 @@
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="F124" t="inlineStr"/>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
       <c r="I124" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>Deutsche Bank Park</t>
         </is>
       </c>
       <c r="J124" t="inlineStr"/>
@@ -4910,59 +4906,59 @@
       <c r="L124" t="inlineStr"/>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>2026-05-02</t>
-        </is>
-      </c>
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>Eintracht Frankfurt</t>
-        </is>
-      </c>
+      <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>Hamburger SV</t>
-        </is>
-      </c>
+      <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr"/>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>Deutsche Bank Park</t>
-        </is>
-      </c>
+      <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
+      <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" t="inlineStr"/>
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2026-05-09</t>
+        </is>
+      </c>
       <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Köln</t>
+        </is>
+      </c>
       <c r="F126" t="inlineStr"/>
-      <c r="G126" t="inlineStr"/>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Heidenheim</t>
+        </is>
+      </c>
       <c r="H126" t="inlineStr"/>
-      <c r="I126" t="inlineStr"/>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>RheinEnergieSTADION</t>
+        </is>
+      </c>
       <c r="J126" t="inlineStr"/>
-      <c r="K126" t="inlineStr"/>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L126" t="inlineStr"/>
     </row>
     <row r="127">
@@ -4984,19 +4980,19 @@
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F127" t="inlineStr"/>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
       <c r="I127" t="inlineStr">
         <is>
-          <t>RheinEnergieSTADION</t>
+          <t>Signal Iduna Park</t>
         </is>
       </c>
       <c r="J127" t="inlineStr"/>
@@ -5026,19 +5022,19 @@
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="F128" t="inlineStr"/>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr">
         <is>
-          <t>Signal Iduna Park</t>
+          <t>Volksparkstadion</t>
         </is>
       </c>
       <c r="J128" t="inlineStr"/>
@@ -5068,19 +5064,19 @@
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>
       <c r="I129" t="inlineStr">
         <is>
-          <t>Volksparkstadion</t>
+          <t>MHPArena</t>
         </is>
       </c>
       <c r="J129" t="inlineStr"/>
@@ -5110,19 +5106,19 @@
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>St Pauli</t>
         </is>
       </c>
       <c r="H130" t="inlineStr"/>
       <c r="I130" t="inlineStr">
         <is>
-          <t>MHPArena</t>
+          <t>Red Bull Arena</t>
         </is>
       </c>
       <c r="J130" t="inlineStr"/>
@@ -5152,19 +5148,19 @@
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="H131" t="inlineStr"/>
       <c r="I131" t="inlineStr">
         <is>
-          <t>Red Bull Arena</t>
+          <t>Mewa Arena</t>
         </is>
       </c>
       <c r="J131" t="inlineStr"/>
@@ -5194,19 +5190,19 @@
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="H132" t="inlineStr"/>
       <c r="I132" t="inlineStr">
         <is>
-          <t>Mewa Arena</t>
+          <t>WWK Arena</t>
         </is>
       </c>
       <c r="J132" t="inlineStr"/>
@@ -5236,19 +5232,19 @@
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="H133" t="inlineStr"/>
       <c r="I133" t="inlineStr">
         <is>
-          <t>WWK Arena</t>
+          <t>PreZero Arena</t>
         </is>
       </c>
       <c r="J133" t="inlineStr"/>
@@ -5278,19 +5274,19 @@
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F134" t="inlineStr"/>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="H134" t="inlineStr"/>
       <c r="I134" t="inlineStr">
         <is>
-          <t>PreZero Arena</t>
+          <t>Volkswagen Arena</t>
         </is>
       </c>
       <c r="J134" t="inlineStr"/>
@@ -5302,59 +5298,63 @@
       <c r="L134" t="inlineStr"/>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>2026-05-09</t>
-        </is>
-      </c>
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
       <c r="D135" t="inlineStr"/>
-      <c r="E135" t="inlineStr">
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
+      <c r="L135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2026-05-16</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>15:30 (10:30)</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>St Pauli</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr"/>
+      <c r="G136" t="inlineStr">
         <is>
           <t>Wolfsburg</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr"/>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>Bayern Munich</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr"/>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>Volkswagen Arena</t>
-        </is>
-      </c>
-      <c r="J135" t="inlineStr"/>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
-      <c r="L135" t="inlineStr"/>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr"/>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
-      <c r="D136" t="inlineStr"/>
-      <c r="E136" t="inlineStr"/>
-      <c r="F136" t="inlineStr"/>
-      <c r="G136" t="inlineStr"/>
       <c r="H136" t="inlineStr"/>
-      <c r="I136" t="inlineStr"/>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>Millerntor-Stadion</t>
+        </is>
+      </c>
       <c r="J136" t="inlineStr"/>
-      <c r="K136" t="inlineStr"/>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>Head-to-Head</t>
+        </is>
+      </c>
       <c r="L136" t="inlineStr"/>
     </row>
     <row r="137">
@@ -5380,19 +5380,19 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>St Pauli</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
       <c r="I137" t="inlineStr">
         <is>
-          <t>Millerntor-Stadion</t>
+          <t>Weserstadion</t>
         </is>
       </c>
       <c r="J137" t="inlineStr"/>
@@ -5426,19 +5426,19 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="F138" t="inlineStr"/>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Mainz 05</t>
         </is>
       </c>
       <c r="H138" t="inlineStr"/>
       <c r="I138" t="inlineStr">
         <is>
-          <t>Weserstadion</t>
+          <t>Voith-Arena</t>
         </is>
       </c>
       <c r="J138" t="inlineStr"/>
@@ -5472,19 +5472,19 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="F139" t="inlineStr"/>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Hamburger SV</t>
         </is>
       </c>
       <c r="H139" t="inlineStr"/>
       <c r="I139" t="inlineStr">
         <is>
-          <t>Voith-Arena</t>
+          <t>BayArena</t>
         </is>
       </c>
       <c r="J139" t="inlineStr"/>
@@ -5518,19 +5518,19 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F140" t="inlineStr"/>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Hamburger SV</t>
+          <t>Köln</t>
         </is>
       </c>
       <c r="H140" t="inlineStr"/>
       <c r="I140" t="inlineStr">
         <is>
-          <t>BayArena</t>
+          <t>Allianz Arena</t>
         </is>
       </c>
       <c r="J140" t="inlineStr"/>
@@ -5564,19 +5564,19 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="F141" t="inlineStr"/>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="H141" t="inlineStr"/>
       <c r="I141" t="inlineStr">
         <is>
-          <t>Allianz Arena</t>
+          <t>Stadion An der Alten Försterei</t>
         </is>
       </c>
       <c r="J141" t="inlineStr"/>
@@ -5610,19 +5610,19 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Gladbach</t>
         </is>
       </c>
       <c r="F142" t="inlineStr"/>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="H142" t="inlineStr"/>
       <c r="I142" t="inlineStr">
         <is>
-          <t>Stadion An der Alten Försterei</t>
+          <t>Stadion im Borussia-Park</t>
         </is>
       </c>
       <c r="J142" t="inlineStr"/>
@@ -5656,19 +5656,19 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Gladbach</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="F143" t="inlineStr"/>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="H143" t="inlineStr"/>
       <c r="I143" t="inlineStr">
         <is>
-          <t>Stadion im Borussia-Park</t>
+          <t>Deutsche Bank Park</t>
         </is>
       </c>
       <c r="J143" t="inlineStr"/>
@@ -5702,19 +5702,19 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F144" t="inlineStr"/>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H144" t="inlineStr"/>
       <c r="I144" t="inlineStr">
         <is>
-          <t>Deutsche Bank Park</t>
+          <t>Europa-Park Stadion</t>
         </is>
       </c>
       <c r="J144" t="inlineStr"/>
@@ -5724,52 +5724,6 @@
         </is>
       </c>
       <c r="L144" t="inlineStr"/>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>2026-05-16</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>15:30 (10:30)</t>
-        </is>
-      </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>Freiburg</t>
-        </is>
-      </c>
-      <c r="F145" t="inlineStr"/>
-      <c r="G145" t="inlineStr">
-        <is>
-          <t>RB Leipzig</t>
-        </is>
-      </c>
-      <c r="H145" t="inlineStr"/>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>Europa-Park Stadion</t>
-        </is>
-      </c>
-      <c r="J145" t="inlineStr"/>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>Head-to-Head</t>
-        </is>
-      </c>
-      <c r="L145" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>